<commit_message>
aggiornati i file excel con la durata totale dei singoli test di download e upload
</commit_message>
<xml_diff>
--- a/GraficiRisultati/100_100/10MB/results.xlsx
+++ b/GraficiRisultati/100_100/10MB/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerongeorge/Documents/RomaTre/Tirocinio/TestLaboratorioFUB/GraficiRisultati/100_100/10MB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerongeorge/Progetto/misurainternet-speedtest/GraficiRisultati/100_100/10MB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,15 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Numero di connessioni</t>
   </si>
   <si>
-    <t>Banda in download</t>
+    <t>Banda in download (Mb/s)</t>
   </si>
   <si>
-    <t>Banda in upload</t>
+    <t>Banda in upload (Mb/s)</t>
+  </si>
+  <si>
+    <t>Tempo totale download (s)</t>
+  </si>
+  <si>
+    <t>Tempo totale upload (s)</t>
   </si>
 </sst>
 </file>
@@ -126,8 +132,22 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Profilo 100/100</a:t>
+              <a:t>Profilo: 100/100</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Dimensione</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> file: 10MB</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -177,7 +197,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Banda in download</c:v>
+                  <c:v>Banda in download (Mb/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -238,7 +258,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Banda in upload</c:v>
+                  <c:v>Banda in upload (Mb/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -300,11 +320,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="5900224"/>
-        <c:axId val="5902000"/>
+        <c:axId val="939825968"/>
+        <c:axId val="939857008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5900224"/>
+        <c:axId val="939825968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,7 +367,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5902000"/>
+        <c:crossAx val="939857008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -355,7 +375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5902000"/>
+        <c:axId val="939857008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +426,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5900224"/>
+        <c:crossAx val="939825968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1034,16 +1054,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1328,15 +1348,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1346,8 +1372,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1357,8 +1389,14 @@
       <c r="C2">
         <v>97.668000000000006</v>
       </c>
+      <c r="D2">
+        <v>16.001999999999999</v>
+      </c>
+      <c r="E2">
+        <v>19.036000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1368,8 +1406,14 @@
       <c r="C3">
         <v>97.481999999999999</v>
       </c>
+      <c r="D3">
+        <v>28.007000000000001</v>
+      </c>
+      <c r="E3">
+        <v>16.052</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1378,6 +1422,12 @@
       </c>
       <c r="C4">
         <v>97.396000000000001</v>
+      </c>
+      <c r="D4">
+        <v>25.001999999999999</v>
+      </c>
+      <c r="E4">
+        <v>16.032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>